<commit_message>
fixed cmake script & results table
</commit_message>
<xml_diff>
--- a/doc/arm-benchmarks-results.xlsx
+++ b/doc/arm-benchmarks-results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianluca/VirtualBox VMs/Shared/nucleo/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianluca/VirtualBox VMs/Shared/arm-nucleo-prolepsis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6EDD52-30F0-7D4C-9242-15C9C1E1E0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3681FA-4F0D-D64D-B292-6914116D8AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3500" yWindow="1740" windowWidth="31220" windowHeight="17440" xr2:uid="{6C163CD9-0266-BA4D-8209-435E9226B323}"/>
   </bookViews>
@@ -128,16 +128,16 @@
     <t>total branches</t>
   </si>
   <si>
-    <t>instr. Percentage</t>
-  </si>
-  <si>
     <t>speed @ 168 MHz (s)</t>
   </si>
   <si>
     <t>GEO</t>
   </si>
   <si>
-    <t>instr. branches</t>
+    <t>prot. branches</t>
+  </si>
+  <si>
+    <t>protection rate</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>28</v>
@@ -625,13 +625,13 @@
         <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>4</v>
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1907,7 +1907,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M26" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N26" s="10">
         <f>GEOMEAN(N2:N23)</f>

</xml_diff>